<commit_message>
DASH vs OpenMM analysis scripts
</commit_message>
<xml_diff>
--- a/Path Integral Simulations.xlsx
+++ b/Path Integral Simulations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swans\Documents\Summer Quarter 2018\Research\Path Integrals\hexane-water\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800F36EB-E04A-481C-8516-5F0F9320F4D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909440A3-7D95-401C-BAD7-C14514F9EE20}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12360" xr2:uid="{F0298022-D4A9-4AA7-A32D-2CC19CDAD08D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>Simulation No.</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Running</t>
   </si>
   <si>
-    <t>Submitted</t>
-  </si>
-  <si>
     <t xml:space="preserve">DASH simulation using run_UPDATE.py and interface_UPDATE.py, filename fulldata-NPT-298, 1M steps equil NPT 298 K 1 atm, 6M steps prod NPT 298 K 1 atm, no PI, data every 10, waldman, restart/traj every 1,000, no z change, no restart.  </t>
   </si>
   <si>
@@ -105,19 +102,64 @@
     <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-1</t>
   </si>
   <si>
-    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MC-1</t>
-  </si>
-  <si>
-    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MC-1</t>
-  </si>
-  <si>
     <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-1</t>
   </si>
   <si>
-    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MM-1</t>
-  </si>
-  <si>
-    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MM-1</t>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MC-2</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MC-3</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MM-2</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MM-3</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 64 bead, data every 1000, restart/traj every 50,000, filename MC-13</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo at 298 K and 1.01325 bar, initial density 0.997, PI 64 bead, data every 1000, restart/traj every 50,000, filename MM-13</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT Berendsen/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename B-1</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT Berendsen/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename B-2</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT Berendsen/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename B-3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT Berendsen/Andersen at 298 K and 1.0 atm, initial density 0.997, PI None, data every 1000, restart/traj every 50,000, filename no-PI-B</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI None, data every 1000, restart/traj every 50,000, filename no-PI-B</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 12 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-4</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 12 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MC-5</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 12 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MC-6</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 1.2 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-4</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 1.2 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MM-5</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 1.2 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MM-6</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -472,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D74D844-A431-4314-9157-676E2445D68B}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -484,7 +526,7 @@
     <col min="2" max="2" width="56.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,228 +537,250 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -724,11 +788,14 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -736,42 +803,199 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
-        <v>3</v>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor change to tip4pF script and updated results
</commit_message>
<xml_diff>
--- a/Path Integral Simulations.xlsx
+++ b/Path Integral Simulations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swans\Documents\Summer Quarter 2018\Research\Path Integrals\hexane-water\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909440A3-7D95-401C-BAD7-C14514F9EE20}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7513A5D-4E26-4E59-93AF-CE4E4C80D914}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12360" xr2:uid="{F0298022-D4A9-4AA7-A32D-2CC19CDAD08D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Simulation No.</t>
   </si>
@@ -138,9 +138,6 @@
     <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT Berendsen/Andersen at 298 K and 1.0 atm, initial density 0.997, PI None, data every 1000, restart/traj every 50,000, filename no-PI-B</t>
   </si>
   <si>
-    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI None, data every 1000, restart/traj every 50,000, filename no-PI-B</t>
-  </si>
-  <si>
     <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 12 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-4</t>
   </si>
   <si>
@@ -160,6 +157,69 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI None, data every 1000, restart/traj every 50,000, filename no-PI-MC</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.25, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-7</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.25, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MC-8</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.25, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MC-9</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.00025 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-7</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.00025 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MM-8</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 4M steps with time step 0.00025 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MM-9</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 1.0, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-10</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 1.0, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MC-11</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 1.0, rCut 9 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MC-12</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 0.001 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-10</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 0.001 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 16 bead, data every 1000, restart/traj every 50,000, filename MM-11</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 1M steps with time step 0.001 ps, rCut 0.9 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.997, PI 32 bead, data every 1000, restart/traj every 50,000, filename MM-12</t>
+  </si>
+  <si>
+    <t>NVT simulation 1 bead OpenMM</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 9 A, NVT Andersen at 298 K, initial density 0.9979734044480487, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-NVT-1bead</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 0.9 nanometers, NVT RPMD/PILE at 298 K, initial density 0.9979734044480487, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-NVT-1bead</t>
+  </si>
+  <si>
+    <t>"" in DASH</t>
+  </si>
+  <si>
+    <t>DASH simulation in dash_work/water using run_9-26-2018.sh and tip4pF_9-26-2018.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.5, rCut 15 A, NPT MonteCarlo/Andersen at 298 K and 1.0 atm, initial density 0.9979734044480487, PI 1 bead, data every 1000, restart/traj every 50,000, filename MC-rCut15</t>
+  </si>
+  <si>
+    <t>Check rCut 15 in DASH</t>
+  </si>
+  <si>
+    <t>OpenMM simulation in /home/swansonk1/openmm using run_openmm.sh and pimd_modified.py, 1000 q-TIP4P/F water molecules, 2M steps with time step 0.0005 ps, rCut 1.5 nanometers, NPT RPMDMonteCarlo/PILE at 298 K and 1.01325 bar, initial density 0.9979734044480487, PI 1 bead, data every 1000, restart/traj every 50,000, filename MM-rCut15</t>
+  </si>
+  <si>
+    <t>Check rCut 15 in OpenMM</t>
   </si>
 </sst>
 </file>
@@ -514,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D74D844-A431-4314-9157-676E2445D68B}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -874,7 +934,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -885,7 +945,10 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -918,7 +981,10 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
@@ -926,10 +992,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
@@ -937,10 +1006,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -948,54 +1020,257 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45">
         <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>